<commit_message>
added wait for invisible
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="240">
   <si>
     <t>Angela</t>
   </si>
@@ -717,6 +717,21 @@
   </si>
   <si>
     <t>0#BHGj3MA</t>
+  </si>
+  <si>
+    <t>Casey</t>
+  </si>
+  <si>
+    <t>Friesen</t>
+  </si>
+  <si>
+    <t>erik.schuppe@example.com</t>
+  </si>
+  <si>
+    <t>&amp;pzZkg</t>
+  </si>
+  <si>
+    <t>09/05/1976</t>
   </si>
 </sst>
 </file>
@@ -761,7 +776,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:E49"/>
+  <dimension ref="A2:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1583,6 +1598,23 @@
         <v>132</v>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>235</v>
+      </c>
+      <c r="B50" t="s">
+        <v>236</v>
+      </c>
+      <c r="C50" t="s">
+        <v>237</v>
+      </c>
+      <c r="D50" t="s">
+        <v>238</v>
+      </c>
+      <c r="E50" t="s">
+        <v>239</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
added Hi Username! verification to SignUpTests and working on LoginTests
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="363">
   <si>
     <t>Angela</t>
   </si>
@@ -1086,6 +1086,21 @@
   </si>
   <si>
     <t>09/27/1991</t>
+  </si>
+  <si>
+    <t>Cliff</t>
+  </si>
+  <si>
+    <t>Fritsch</t>
+  </si>
+  <si>
+    <t>alberto.gulgowski@example.com</t>
+  </si>
+  <si>
+    <t>DO5LaP%mZ</t>
+  </si>
+  <si>
+    <t>04/16/1979</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1145,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:E74"/>
+  <dimension ref="A2:E75"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -2377,6 +2392,23 @@
         <v>357</v>
       </c>
     </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>358</v>
+      </c>
+      <c r="B75" t="s">
+        <v>359</v>
+      </c>
+      <c r="C75" t="s">
+        <v>360</v>
+      </c>
+      <c r="D75" t="s">
+        <v>361</v>
+      </c>
+      <c r="E75" t="s">
+        <v>362</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
adding AccountPage to validate user data
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="403">
   <si>
     <t>Angela</t>
   </si>
@@ -1101,6 +1101,126 @@
   </si>
   <si>
     <t>04/16/1979</t>
+  </si>
+  <si>
+    <t>Albertine</t>
+  </si>
+  <si>
+    <t>Gorczany</t>
+  </si>
+  <si>
+    <t>marlon.koepp@example.com</t>
+  </si>
+  <si>
+    <t>4a6tK!2&amp;klW</t>
+  </si>
+  <si>
+    <t>01/27/1981</t>
+  </si>
+  <si>
+    <t>Lacresha</t>
+  </si>
+  <si>
+    <t>Johnston</t>
+  </si>
+  <si>
+    <t>youlanda.carter@example.com</t>
+  </si>
+  <si>
+    <t>^$iI7I</t>
+  </si>
+  <si>
+    <t>07/24/1991</t>
+  </si>
+  <si>
+    <t>Glenn</t>
+  </si>
+  <si>
+    <t>Zemlak</t>
+  </si>
+  <si>
+    <t>loris.padberg@example.com</t>
+  </si>
+  <si>
+    <t>JRF4094AF</t>
+  </si>
+  <si>
+    <t>09/04/1956</t>
+  </si>
+  <si>
+    <t>Johnnie</t>
+  </si>
+  <si>
+    <t>Toy</t>
+  </si>
+  <si>
+    <t>deloise.hammes@example.com</t>
+  </si>
+  <si>
+    <t>4Ig7NHH4c</t>
+  </si>
+  <si>
+    <t>05/29/1986</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Mills</t>
+  </si>
+  <si>
+    <t>jamison.olson@example.com</t>
+  </si>
+  <si>
+    <t>&amp;*@3X9@d</t>
+  </si>
+  <si>
+    <t>01/05/1967</t>
+  </si>
+  <si>
+    <t>Brice</t>
+  </si>
+  <si>
+    <t>Will</t>
+  </si>
+  <si>
+    <t>emmie.fahey@example.com</t>
+  </si>
+  <si>
+    <t>zsRV#sjw</t>
+  </si>
+  <si>
+    <t>10/04/1982</t>
+  </si>
+  <si>
+    <t>Beaulah</t>
+  </si>
+  <si>
+    <t>Lehner</t>
+  </si>
+  <si>
+    <t>ka.corkery@example.com</t>
+  </si>
+  <si>
+    <t>7Tb4139KuA</t>
+  </si>
+  <si>
+    <t>06/11/1988</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Reichert</t>
+  </si>
+  <si>
+    <t>garry.mccullough@example.com</t>
+  </si>
+  <si>
+    <t>2#v@3x1</t>
+  </si>
+  <si>
+    <t>01/22/1964</t>
   </si>
 </sst>
 </file>
@@ -1145,7 +1265,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:E75"/>
+  <dimension ref="A2:E83"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -2409,6 +2529,142 @@
         <v>362</v>
       </c>
     </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>363</v>
+      </c>
+      <c r="B76" t="s">
+        <v>364</v>
+      </c>
+      <c r="C76" t="s">
+        <v>365</v>
+      </c>
+      <c r="D76" t="s">
+        <v>366</v>
+      </c>
+      <c r="E76" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>368</v>
+      </c>
+      <c r="B77" t="s">
+        <v>369</v>
+      </c>
+      <c r="C77" t="s">
+        <v>370</v>
+      </c>
+      <c r="D77" t="s">
+        <v>371</v>
+      </c>
+      <c r="E77" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>373</v>
+      </c>
+      <c r="B78" t="s">
+        <v>374</v>
+      </c>
+      <c r="C78" t="s">
+        <v>375</v>
+      </c>
+      <c r="D78" t="s">
+        <v>376</v>
+      </c>
+      <c r="E78" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>378</v>
+      </c>
+      <c r="B79" t="s">
+        <v>379</v>
+      </c>
+      <c r="C79" t="s">
+        <v>380</v>
+      </c>
+      <c r="D79" t="s">
+        <v>381</v>
+      </c>
+      <c r="E79" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>383</v>
+      </c>
+      <c r="B80" t="s">
+        <v>384</v>
+      </c>
+      <c r="C80" t="s">
+        <v>385</v>
+      </c>
+      <c r="D80" t="s">
+        <v>386</v>
+      </c>
+      <c r="E80" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>388</v>
+      </c>
+      <c r="B81" t="s">
+        <v>389</v>
+      </c>
+      <c r="C81" t="s">
+        <v>390</v>
+      </c>
+      <c r="D81" t="s">
+        <v>391</v>
+      </c>
+      <c r="E81" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>393</v>
+      </c>
+      <c r="B82" t="s">
+        <v>394</v>
+      </c>
+      <c r="C82" t="s">
+        <v>395</v>
+      </c>
+      <c r="D82" t="s">
+        <v>396</v>
+      </c>
+      <c r="E82" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>398</v>
+      </c>
+      <c r="B83" t="s">
+        <v>399</v>
+      </c>
+      <c r="C83" t="s">
+        <v>400</v>
+      </c>
+      <c r="D83" t="s">
+        <v>401</v>
+      </c>
+      <c r="E83" t="s">
+        <v>402</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>